<commit_message>
Corrections noms classes mapping 896da81aef82b3a0d51ef0d7414498d600b3b18a
</commit_message>
<xml_diff>
--- a/305-mapping---ajouter-un-mapping-technique-fonctionnel/ig/StructureDefinition-tddui-Encounter-sejour.xlsx
+++ b/305-mapping---ajouter-un-mapping-technique-fonctionnel/ig/StructureDefinition-tddui-Encounter-sejour.xlsx
@@ -57,7 +57,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2025-07-25T13:53:43+00:00</t>
+    <t>2025-07-28T11:47:16+00:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -1826,7 +1826,7 @@
     <t>The organization that is primarily responsible for this Encounter's services. This MAY be the same as the organization on the Patient record, however it could be different, such as if the actor performing the services was from an external organization (which may be billed seperately) for an external consultation.  Refer to the example bundle showing an abbreviated set of Encounters for a colonoscopy.</t>
   </si>
   <si>
-    <t>ESSMS</t>
+    <t>EntiteJuridique</t>
   </si>
   <si>
     <t>.particiaption[typeCode=PFM].role</t>

</xml_diff>

<commit_message>
Ajout schémas mapping et corrections cad630402ad44d7f5f9d34136d75e38f4c9d30f5
</commit_message>
<xml_diff>
--- a/305-mapping---ajouter-un-mapping-technique-fonctionnel/ig/StructureDefinition-tddui-Encounter-sejour.xlsx
+++ b/305-mapping---ajouter-un-mapping-technique-fonctionnel/ig/StructureDefinition-tddui-Encounter-sejour.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3451" uniqueCount="593">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3451" uniqueCount="594">
   <si>
     <t>Property</t>
   </si>
@@ -57,7 +57,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2025-07-28T11:47:16+00:00</t>
+    <t>2025-07-28T13:00:34+00:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -234,7 +234,7 @@
     <t>Constraint(s)</t>
   </si>
   <si>
-    <t xml:space="preserve">Mapping: Séjours </t>
+    <t>Mapping: Modèle de contenu DUI</t>
   </si>
   <si>
     <t>Mapping: Workflow Pattern</t>
@@ -514,7 +514,7 @@
     <t>Date d’admission dans la structure ESSMS.</t>
   </si>
   <si>
-    <t>dateEntree</t>
+    <t>dateAdmission</t>
   </si>
   <si>
     <t>Encounter.extension:TDDUIEntryModelabel</t>
@@ -1322,6 +1322,9 @@
   <si>
     <t xml:space="preserve">per-1
 </t>
+  </si>
+  <si>
+    <t>dateEntree</t>
   </si>
   <si>
     <t>./low</t>
@@ -2205,7 +2208,7 @@
     <col min="33" max="33" width="9.046875" customWidth="true" bestFit="true" hidden="true"/>
     <col min="34" max="34" width="9.46484375" customWidth="true" bestFit="true"/>
     <col min="35" max="35" width="100.703125" customWidth="true"/>
-    <col min="37" max="37" width="20.5703125" customWidth="true" bestFit="true"/>
+    <col min="37" max="37" width="30.4765625" customWidth="true" bestFit="true"/>
     <col min="38" max="38" width="25.4609375" customWidth="true" bestFit="true"/>
     <col min="39" max="39" width="87.9765625" customWidth="true" bestFit="true"/>
     <col min="40" max="40" width="31.65234375" customWidth="true" bestFit="true"/>
@@ -8953,27 +8956,27 @@
         <v>102</v>
       </c>
       <c r="AK58" t="s" s="2">
-        <v>160</v>
+        <v>420</v>
       </c>
       <c r="AL58" t="s" s="2">
         <v>81</v>
       </c>
       <c r="AM58" t="s" s="2">
-        <v>420</v>
+        <v>421</v>
       </c>
       <c r="AN58" t="s" s="2">
         <v>81</v>
       </c>
       <c r="AO58" t="s" s="2">
-        <v>421</v>
+        <v>422</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="s" s="2">
-        <v>422</v>
+        <v>423</v>
       </c>
       <c r="B59" t="s" s="2">
-        <v>422</v>
+        <v>423</v>
       </c>
       <c r="C59" s="2"/>
       <c r="D59" t="s" s="2">
@@ -8999,20 +9002,20 @@
         <v>414</v>
       </c>
       <c r="L59" t="s" s="2">
-        <v>423</v>
+        <v>424</v>
       </c>
       <c r="M59" t="s" s="2">
-        <v>424</v>
+        <v>425</v>
       </c>
       <c r="N59" t="s" s="2">
-        <v>425</v>
+        <v>426</v>
       </c>
       <c r="O59" s="2"/>
       <c r="P59" t="s" s="2">
         <v>81</v>
       </c>
       <c r="Q59" t="s" s="2">
-        <v>426</v>
+        <v>427</v>
       </c>
       <c r="R59" t="s" s="2">
         <v>81</v>
@@ -9057,7 +9060,7 @@
         <v>81</v>
       </c>
       <c r="AF59" t="s" s="2">
-        <v>427</v>
+        <v>428</v>
       </c>
       <c r="AG59" t="s" s="2">
         <v>79</v>
@@ -9072,27 +9075,27 @@
         <v>102</v>
       </c>
       <c r="AK59" t="s" s="2">
-        <v>428</v>
+        <v>429</v>
       </c>
       <c r="AL59" t="s" s="2">
         <v>81</v>
       </c>
       <c r="AM59" t="s" s="2">
-        <v>429</v>
+        <v>430</v>
       </c>
       <c r="AN59" t="s" s="2">
         <v>81</v>
       </c>
       <c r="AO59" t="s" s="2">
-        <v>430</v>
+        <v>431</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="s" s="2">
-        <v>431</v>
+        <v>432</v>
       </c>
       <c r="B60" t="s" s="2">
-        <v>431</v>
+        <v>432</v>
       </c>
       <c r="C60" s="2"/>
       <c r="D60" t="s" s="2">
@@ -9115,16 +9118,16 @@
         <v>81</v>
       </c>
       <c r="K60" t="s" s="2">
-        <v>432</v>
+        <v>433</v>
       </c>
       <c r="L60" t="s" s="2">
-        <v>433</v>
+        <v>434</v>
       </c>
       <c r="M60" t="s" s="2">
-        <v>434</v>
+        <v>435</v>
       </c>
       <c r="N60" t="s" s="2">
-        <v>435</v>
+        <v>436</v>
       </c>
       <c r="O60" s="2"/>
       <c r="P60" t="s" s="2">
@@ -9174,7 +9177,7 @@
         <v>81</v>
       </c>
       <c r="AF60" t="s" s="2">
-        <v>431</v>
+        <v>432</v>
       </c>
       <c r="AG60" t="s" s="2">
         <v>79</v>
@@ -9195,25 +9198,25 @@
         <v>407</v>
       </c>
       <c r="AM60" t="s" s="2">
-        <v>436</v>
+        <v>437</v>
       </c>
       <c r="AN60" t="s" s="2">
         <v>81</v>
       </c>
       <c r="AO60" t="s" s="2">
-        <v>437</v>
+        <v>438</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="s" s="2">
-        <v>438</v>
+        <v>439</v>
       </c>
       <c r="B61" t="s" s="2">
-        <v>438</v>
+        <v>439</v>
       </c>
       <c r="C61" s="2"/>
       <c r="D61" t="s" s="2">
-        <v>439</v>
+        <v>440</v>
       </c>
       <c r="E61" s="2"/>
       <c r="F61" t="s" s="2">
@@ -9235,13 +9238,13 @@
         <v>225</v>
       </c>
       <c r="L61" t="s" s="2">
-        <v>440</v>
+        <v>441</v>
       </c>
       <c r="M61" t="s" s="2">
-        <v>441</v>
+        <v>442</v>
       </c>
       <c r="N61" t="s" s="2">
-        <v>442</v>
+        <v>443</v>
       </c>
       <c r="O61" s="2"/>
       <c r="P61" t="s" s="2">
@@ -9270,10 +9273,10 @@
         <v>114</v>
       </c>
       <c r="Y61" t="s" s="2">
-        <v>443</v>
+        <v>444</v>
       </c>
       <c r="Z61" t="s" s="2">
-        <v>444</v>
+        <v>445</v>
       </c>
       <c r="AA61" t="s" s="2">
         <v>81</v>
@@ -9291,7 +9294,7 @@
         <v>81</v>
       </c>
       <c r="AF61" t="s" s="2">
-        <v>438</v>
+        <v>439</v>
       </c>
       <c r="AG61" t="s" s="2">
         <v>79</v>
@@ -9309,28 +9312,28 @@
         <v>81</v>
       </c>
       <c r="AL61" t="s" s="2">
-        <v>445</v>
+        <v>446</v>
       </c>
       <c r="AM61" t="s" s="2">
-        <v>446</v>
+        <v>447</v>
       </c>
       <c r="AN61" t="s" s="2">
-        <v>447</v>
+        <v>448</v>
       </c>
       <c r="AO61" t="s" s="2">
-        <v>448</v>
+        <v>449</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="s" s="2">
-        <v>449</v>
+        <v>450</v>
       </c>
       <c r="B62" t="s" s="2">
-        <v>449</v>
+        <v>450</v>
       </c>
       <c r="C62" s="2"/>
       <c r="D62" t="s" s="2">
-        <v>439</v>
+        <v>440</v>
       </c>
       <c r="E62" s="2"/>
       <c r="F62" t="s" s="2">
@@ -9349,16 +9352,16 @@
         <v>91</v>
       </c>
       <c r="K62" t="s" s="2">
-        <v>450</v>
+        <v>451</v>
       </c>
       <c r="L62" t="s" s="2">
-        <v>451</v>
+        <v>452</v>
       </c>
       <c r="M62" t="s" s="2">
-        <v>441</v>
+        <v>442</v>
       </c>
       <c r="N62" t="s" s="2">
-        <v>442</v>
+        <v>443</v>
       </c>
       <c r="O62" s="2"/>
       <c r="P62" t="s" s="2">
@@ -9408,7 +9411,7 @@
         <v>81</v>
       </c>
       <c r="AF62" t="s" s="2">
-        <v>449</v>
+        <v>450</v>
       </c>
       <c r="AG62" t="s" s="2">
         <v>79</v>
@@ -9426,24 +9429,24 @@
         <v>81</v>
       </c>
       <c r="AL62" t="s" s="2">
-        <v>445</v>
+        <v>446</v>
       </c>
       <c r="AM62" t="s" s="2">
-        <v>446</v>
+        <v>447</v>
       </c>
       <c r="AN62" t="s" s="2">
-        <v>447</v>
+        <v>448</v>
       </c>
       <c r="AO62" t="s" s="2">
-        <v>448</v>
+        <v>449</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="s" s="2">
-        <v>452</v>
+        <v>453</v>
       </c>
       <c r="B63" t="s" s="2">
-        <v>452</v>
+        <v>453</v>
       </c>
       <c r="C63" s="2"/>
       <c r="D63" t="s" s="2">
@@ -9469,10 +9472,10 @@
         <v>283</v>
       </c>
       <c r="L63" t="s" s="2">
-        <v>453</v>
+        <v>454</v>
       </c>
       <c r="M63" t="s" s="2">
-        <v>454</v>
+        <v>455</v>
       </c>
       <c r="N63" s="2"/>
       <c r="O63" s="2"/>
@@ -9523,7 +9526,7 @@
         <v>81</v>
       </c>
       <c r="AF63" t="s" s="2">
-        <v>452</v>
+        <v>453</v>
       </c>
       <c r="AG63" t="s" s="2">
         <v>79</v>
@@ -9544,7 +9547,7 @@
         <v>81</v>
       </c>
       <c r="AM63" t="s" s="2">
-        <v>455</v>
+        <v>456</v>
       </c>
       <c r="AN63" t="s" s="2">
         <v>81</v>
@@ -9555,10 +9558,10 @@
     </row>
     <row r="64">
       <c r="A64" t="s" s="2">
-        <v>456</v>
+        <v>457</v>
       </c>
       <c r="B64" t="s" s="2">
-        <v>456</v>
+        <v>457</v>
       </c>
       <c r="C64" s="2"/>
       <c r="D64" t="s" s="2">
@@ -9670,10 +9673,10 @@
     </row>
     <row r="65">
       <c r="A65" t="s" s="2">
-        <v>457</v>
+        <v>458</v>
       </c>
       <c r="B65" t="s" s="2">
-        <v>457</v>
+        <v>458</v>
       </c>
       <c r="C65" s="2"/>
       <c r="D65" t="s" s="2">
@@ -9787,10 +9790,10 @@
     </row>
     <row r="66">
       <c r="A66" t="s" s="2">
-        <v>458</v>
+        <v>459</v>
       </c>
       <c r="B66" t="s" s="2">
-        <v>458</v>
+        <v>459</v>
       </c>
       <c r="C66" s="2"/>
       <c r="D66" t="s" s="2">
@@ -9906,14 +9909,14 @@
     </row>
     <row r="67">
       <c r="A67" t="s" s="2">
-        <v>459</v>
+        <v>460</v>
       </c>
       <c r="B67" t="s" s="2">
-        <v>459</v>
+        <v>460</v>
       </c>
       <c r="C67" s="2"/>
       <c r="D67" t="s" s="2">
-        <v>460</v>
+        <v>461</v>
       </c>
       <c r="E67" s="2"/>
       <c r="F67" t="s" s="2">
@@ -9932,16 +9935,16 @@
         <v>91</v>
       </c>
       <c r="K67" t="s" s="2">
-        <v>461</v>
+        <v>462</v>
       </c>
       <c r="L67" t="s" s="2">
-        <v>462</v>
+        <v>463</v>
       </c>
       <c r="M67" t="s" s="2">
-        <v>463</v>
+        <v>464</v>
       </c>
       <c r="N67" t="s" s="2">
-        <v>442</v>
+        <v>443</v>
       </c>
       <c r="O67" s="2"/>
       <c r="P67" t="s" s="2">
@@ -9991,7 +9994,7 @@
         <v>81</v>
       </c>
       <c r="AF67" t="s" s="2">
-        <v>459</v>
+        <v>460</v>
       </c>
       <c r="AG67" t="s" s="2">
         <v>90</v>
@@ -10009,24 +10012,24 @@
         <v>81</v>
       </c>
       <c r="AL67" t="s" s="2">
-        <v>464</v>
+        <v>465</v>
       </c>
       <c r="AM67" t="s" s="2">
-        <v>465</v>
+        <v>466</v>
       </c>
       <c r="AN67" t="s" s="2">
-        <v>447</v>
+        <v>448</v>
       </c>
       <c r="AO67" t="s" s="2">
-        <v>466</v>
+        <v>467</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="s" s="2">
-        <v>467</v>
+        <v>468</v>
       </c>
       <c r="B68" t="s" s="2">
-        <v>467</v>
+        <v>468</v>
       </c>
       <c r="C68" s="2"/>
       <c r="D68" t="s" s="2">
@@ -10052,10 +10055,10 @@
         <v>225</v>
       </c>
       <c r="L68" t="s" s="2">
-        <v>468</v>
+        <v>469</v>
       </c>
       <c r="M68" t="s" s="2">
-        <v>469</v>
+        <v>470</v>
       </c>
       <c r="N68" s="2"/>
       <c r="O68" s="2"/>
@@ -10085,10 +10088,10 @@
         <v>114</v>
       </c>
       <c r="Y68" t="s" s="2">
-        <v>470</v>
+        <v>471</v>
       </c>
       <c r="Z68" t="s" s="2">
-        <v>471</v>
+        <v>472</v>
       </c>
       <c r="AA68" t="s" s="2">
         <v>81</v>
@@ -10106,7 +10109,7 @@
         <v>81</v>
       </c>
       <c r="AF68" t="s" s="2">
-        <v>467</v>
+        <v>468</v>
       </c>
       <c r="AG68" t="s" s="2">
         <v>79</v>
@@ -10138,10 +10141,10 @@
     </row>
     <row r="69">
       <c r="A69" t="s" s="2">
-        <v>472</v>
+        <v>473</v>
       </c>
       <c r="B69" t="s" s="2">
-        <v>472</v>
+        <v>473</v>
       </c>
       <c r="C69" s="2"/>
       <c r="D69" t="s" s="2">
@@ -10164,13 +10167,13 @@
         <v>81</v>
       </c>
       <c r="K69" t="s" s="2">
-        <v>473</v>
+        <v>474</v>
       </c>
       <c r="L69" t="s" s="2">
-        <v>474</v>
+        <v>475</v>
       </c>
       <c r="M69" t="s" s="2">
-        <v>475</v>
+        <v>476</v>
       </c>
       <c r="N69" s="2"/>
       <c r="O69" s="2"/>
@@ -10221,7 +10224,7 @@
         <v>81</v>
       </c>
       <c r="AF69" t="s" s="2">
-        <v>472</v>
+        <v>473</v>
       </c>
       <c r="AG69" t="s" s="2">
         <v>79</v>
@@ -10242,7 +10245,7 @@
         <v>81</v>
       </c>
       <c r="AM69" t="s" s="2">
-        <v>476</v>
+        <v>477</v>
       </c>
       <c r="AN69" t="s" s="2">
         <v>81</v>
@@ -10253,10 +10256,10 @@
     </row>
     <row r="70">
       <c r="A70" t="s" s="2">
-        <v>477</v>
+        <v>478</v>
       </c>
       <c r="B70" t="s" s="2">
-        <v>477</v>
+        <v>478</v>
       </c>
       <c r="C70" s="2"/>
       <c r="D70" t="s" s="2">
@@ -10279,16 +10282,16 @@
         <v>81</v>
       </c>
       <c r="K70" t="s" s="2">
-        <v>478</v>
+        <v>479</v>
       </c>
       <c r="L70" t="s" s="2">
-        <v>479</v>
+        <v>480</v>
       </c>
       <c r="M70" t="s" s="2">
-        <v>480</v>
+        <v>481</v>
       </c>
       <c r="N70" t="s" s="2">
-        <v>481</v>
+        <v>482</v>
       </c>
       <c r="O70" s="2"/>
       <c r="P70" t="s" s="2">
@@ -10338,7 +10341,7 @@
         <v>81</v>
       </c>
       <c r="AF70" t="s" s="2">
-        <v>477</v>
+        <v>478</v>
       </c>
       <c r="AG70" t="s" s="2">
         <v>79</v>
@@ -10359,7 +10362,7 @@
         <v>81</v>
       </c>
       <c r="AM70" t="s" s="2">
-        <v>482</v>
+        <v>483</v>
       </c>
       <c r="AN70" t="s" s="2">
         <v>81</v>
@@ -10370,10 +10373,10 @@
     </row>
     <row r="71">
       <c r="A71" t="s" s="2">
-        <v>483</v>
+        <v>484</v>
       </c>
       <c r="B71" t="s" s="2">
-        <v>483</v>
+        <v>484</v>
       </c>
       <c r="C71" s="2"/>
       <c r="D71" t="s" s="2">
@@ -10399,13 +10402,13 @@
         <v>283</v>
       </c>
       <c r="L71" t="s" s="2">
-        <v>484</v>
+        <v>485</v>
       </c>
       <c r="M71" t="s" s="2">
-        <v>485</v>
+        <v>486</v>
       </c>
       <c r="N71" t="s" s="2">
-        <v>486</v>
+        <v>487</v>
       </c>
       <c r="O71" s="2"/>
       <c r="P71" t="s" s="2">
@@ -10455,7 +10458,7 @@
         <v>81</v>
       </c>
       <c r="AF71" t="s" s="2">
-        <v>483</v>
+        <v>484</v>
       </c>
       <c r="AG71" t="s" s="2">
         <v>79</v>
@@ -10476,7 +10479,7 @@
         <v>81</v>
       </c>
       <c r="AM71" t="s" s="2">
-        <v>487</v>
+        <v>488</v>
       </c>
       <c r="AN71" t="s" s="2">
         <v>81</v>
@@ -10487,10 +10490,10 @@
     </row>
     <row r="72">
       <c r="A72" t="s" s="2">
-        <v>488</v>
+        <v>489</v>
       </c>
       <c r="B72" t="s" s="2">
-        <v>488</v>
+        <v>489</v>
       </c>
       <c r="C72" s="2"/>
       <c r="D72" t="s" s="2">
@@ -10602,10 +10605,10 @@
     </row>
     <row r="73">
       <c r="A73" t="s" s="2">
-        <v>489</v>
+        <v>490</v>
       </c>
       <c r="B73" t="s" s="2">
-        <v>489</v>
+        <v>490</v>
       </c>
       <c r="C73" s="2"/>
       <c r="D73" t="s" s="2">
@@ -10719,10 +10722,10 @@
     </row>
     <row r="74">
       <c r="A74" t="s" s="2">
-        <v>490</v>
+        <v>491</v>
       </c>
       <c r="B74" t="s" s="2">
-        <v>490</v>
+        <v>491</v>
       </c>
       <c r="C74" s="2"/>
       <c r="D74" t="s" s="2">
@@ -10838,10 +10841,10 @@
     </row>
     <row r="75">
       <c r="A75" t="s" s="2">
-        <v>491</v>
+        <v>492</v>
       </c>
       <c r="B75" t="s" s="2">
-        <v>491</v>
+        <v>492</v>
       </c>
       <c r="C75" s="2"/>
       <c r="D75" t="s" s="2">
@@ -10867,10 +10870,10 @@
         <v>187</v>
       </c>
       <c r="L75" t="s" s="2">
-        <v>492</v>
+        <v>493</v>
       </c>
       <c r="M75" t="s" s="2">
-        <v>493</v>
+        <v>494</v>
       </c>
       <c r="N75" s="2"/>
       <c r="O75" s="2"/>
@@ -10921,7 +10924,7 @@
         <v>81</v>
       </c>
       <c r="AF75" t="s" s="2">
-        <v>491</v>
+        <v>492</v>
       </c>
       <c r="AG75" t="s" s="2">
         <v>79</v>
@@ -10948,15 +10951,15 @@
         <v>81</v>
       </c>
       <c r="AO75" t="s" s="2">
-        <v>494</v>
+        <v>495</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="s" s="2">
-        <v>495</v>
+        <v>496</v>
       </c>
       <c r="B76" t="s" s="2">
-        <v>495</v>
+        <v>496</v>
       </c>
       <c r="C76" s="2"/>
       <c r="D76" t="s" s="2">
@@ -10979,13 +10982,13 @@
         <v>81</v>
       </c>
       <c r="K76" t="s" s="2">
-        <v>496</v>
+        <v>497</v>
       </c>
       <c r="L76" t="s" s="2">
-        <v>497</v>
+        <v>498</v>
       </c>
       <c r="M76" t="s" s="2">
-        <v>498</v>
+        <v>499</v>
       </c>
       <c r="N76" s="2"/>
       <c r="O76" s="2"/>
@@ -11036,7 +11039,7 @@
         <v>81</v>
       </c>
       <c r="AF76" t="s" s="2">
-        <v>495</v>
+        <v>496</v>
       </c>
       <c r="AG76" t="s" s="2">
         <v>79</v>
@@ -11057,7 +11060,7 @@
         <v>81</v>
       </c>
       <c r="AM76" t="s" s="2">
-        <v>499</v>
+        <v>500</v>
       </c>
       <c r="AN76" t="s" s="2">
         <v>81</v>
@@ -11068,10 +11071,10 @@
     </row>
     <row r="77">
       <c r="A77" t="s" s="2">
-        <v>500</v>
+        <v>501</v>
       </c>
       <c r="B77" t="s" s="2">
-        <v>500</v>
+        <v>501</v>
       </c>
       <c r="C77" s="2"/>
       <c r="D77" t="s" s="2">
@@ -11097,10 +11100,10 @@
         <v>225</v>
       </c>
       <c r="L77" t="s" s="2">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="M77" t="s" s="2">
-        <v>502</v>
+        <v>503</v>
       </c>
       <c r="N77" s="2"/>
       <c r="O77" s="2"/>
@@ -11130,10 +11133,10 @@
         <v>114</v>
       </c>
       <c r="Y77" t="s" s="2">
-        <v>503</v>
+        <v>504</v>
       </c>
       <c r="Z77" t="s" s="2">
-        <v>504</v>
+        <v>505</v>
       </c>
       <c r="AA77" t="s" s="2">
         <v>81</v>
@@ -11151,7 +11154,7 @@
         <v>81</v>
       </c>
       <c r="AF77" t="s" s="2">
-        <v>500</v>
+        <v>501</v>
       </c>
       <c r="AG77" t="s" s="2">
         <v>79</v>
@@ -11172,21 +11175,21 @@
         <v>81</v>
       </c>
       <c r="AM77" t="s" s="2">
-        <v>505</v>
+        <v>506</v>
       </c>
       <c r="AN77" t="s" s="2">
         <v>81</v>
       </c>
       <c r="AO77" t="s" s="2">
-        <v>506</v>
+        <v>507</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="s" s="2">
-        <v>507</v>
+        <v>508</v>
       </c>
       <c r="B78" t="s" s="2">
-        <v>507</v>
+        <v>508</v>
       </c>
       <c r="C78" s="2"/>
       <c r="D78" t="s" s="2">
@@ -11212,10 +11215,10 @@
         <v>225</v>
       </c>
       <c r="L78" t="s" s="2">
-        <v>508</v>
+        <v>509</v>
       </c>
       <c r="M78" t="s" s="2">
-        <v>509</v>
+        <v>510</v>
       </c>
       <c r="N78" s="2"/>
       <c r="O78" s="2"/>
@@ -11245,10 +11248,10 @@
         <v>323</v>
       </c>
       <c r="Y78" t="s" s="2">
-        <v>510</v>
+        <v>511</v>
       </c>
       <c r="Z78" t="s" s="2">
-        <v>511</v>
+        <v>512</v>
       </c>
       <c r="AA78" t="s" s="2">
         <v>81</v>
@@ -11266,7 +11269,7 @@
         <v>81</v>
       </c>
       <c r="AF78" t="s" s="2">
-        <v>507</v>
+        <v>508</v>
       </c>
       <c r="AG78" t="s" s="2">
         <v>79</v>
@@ -11293,15 +11296,15 @@
         <v>81</v>
       </c>
       <c r="AO78" t="s" s="2">
-        <v>512</v>
+        <v>513</v>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="s" s="2">
-        <v>513</v>
+        <v>514</v>
       </c>
       <c r="B79" t="s" s="2">
-        <v>513</v>
+        <v>514</v>
       </c>
       <c r="C79" s="2"/>
       <c r="D79" t="s" s="2">
@@ -11327,16 +11330,16 @@
         <v>225</v>
       </c>
       <c r="L79" t="s" s="2">
-        <v>514</v>
+        <v>515</v>
       </c>
       <c r="M79" t="s" s="2">
-        <v>515</v>
+        <v>516</v>
       </c>
       <c r="N79" t="s" s="2">
-        <v>516</v>
+        <v>517</v>
       </c>
       <c r="O79" t="s" s="2">
-        <v>517</v>
+        <v>518</v>
       </c>
       <c r="P79" t="s" s="2">
         <v>81</v>
@@ -11364,10 +11367,10 @@
         <v>323</v>
       </c>
       <c r="Y79" t="s" s="2">
-        <v>518</v>
+        <v>519</v>
       </c>
       <c r="Z79" t="s" s="2">
-        <v>519</v>
+        <v>520</v>
       </c>
       <c r="AA79" t="s" s="2">
         <v>81</v>
@@ -11385,7 +11388,7 @@
         <v>81</v>
       </c>
       <c r="AF79" t="s" s="2">
-        <v>513</v>
+        <v>514</v>
       </c>
       <c r="AG79" t="s" s="2">
         <v>79</v>
@@ -11406,21 +11409,21 @@
         <v>81</v>
       </c>
       <c r="AM79" t="s" s="2">
-        <v>520</v>
+        <v>521</v>
       </c>
       <c r="AN79" t="s" s="2">
         <v>81</v>
       </c>
       <c r="AO79" t="s" s="2">
-        <v>521</v>
+        <v>522</v>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="s" s="2">
-        <v>522</v>
+        <v>523</v>
       </c>
       <c r="B80" t="s" s="2">
-        <v>522</v>
+        <v>523</v>
       </c>
       <c r="C80" s="2"/>
       <c r="D80" t="s" s="2">
@@ -11446,10 +11449,10 @@
         <v>225</v>
       </c>
       <c r="L80" t="s" s="2">
-        <v>523</v>
+        <v>524</v>
       </c>
       <c r="M80" t="s" s="2">
-        <v>524</v>
+        <v>525</v>
       </c>
       <c r="N80" s="2"/>
       <c r="O80" s="2"/>
@@ -11479,10 +11482,10 @@
         <v>114</v>
       </c>
       <c r="Y80" t="s" s="2">
-        <v>525</v>
+        <v>526</v>
       </c>
       <c r="Z80" t="s" s="2">
-        <v>526</v>
+        <v>527</v>
       </c>
       <c r="AA80" t="s" s="2">
         <v>81</v>
@@ -11500,7 +11503,7 @@
         <v>81</v>
       </c>
       <c r="AF80" t="s" s="2">
-        <v>522</v>
+        <v>523</v>
       </c>
       <c r="AG80" t="s" s="2">
         <v>79</v>
@@ -11521,21 +11524,21 @@
         <v>81</v>
       </c>
       <c r="AM80" t="s" s="2">
-        <v>527</v>
+        <v>528</v>
       </c>
       <c r="AN80" t="s" s="2">
         <v>81</v>
       </c>
       <c r="AO80" t="s" s="2">
-        <v>528</v>
+        <v>529</v>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="s" s="2">
-        <v>529</v>
+        <v>530</v>
       </c>
       <c r="B81" t="s" s="2">
-        <v>529</v>
+        <v>530</v>
       </c>
       <c r="C81" s="2"/>
       <c r="D81" t="s" s="2">
@@ -11561,10 +11564,10 @@
         <v>225</v>
       </c>
       <c r="L81" t="s" s="2">
-        <v>530</v>
+        <v>531</v>
       </c>
       <c r="M81" t="s" s="2">
-        <v>531</v>
+        <v>532</v>
       </c>
       <c r="N81" s="2"/>
       <c r="O81" s="2"/>
@@ -11594,10 +11597,10 @@
         <v>114</v>
       </c>
       <c r="Y81" t="s" s="2">
-        <v>532</v>
+        <v>533</v>
       </c>
       <c r="Z81" t="s" s="2">
-        <v>533</v>
+        <v>534</v>
       </c>
       <c r="AA81" t="s" s="2">
         <v>81</v>
@@ -11615,7 +11618,7 @@
         <v>81</v>
       </c>
       <c r="AF81" t="s" s="2">
-        <v>529</v>
+        <v>530</v>
       </c>
       <c r="AG81" t="s" s="2">
         <v>79</v>
@@ -11636,21 +11639,21 @@
         <v>81</v>
       </c>
       <c r="AM81" t="s" s="2">
-        <v>534</v>
+        <v>535</v>
       </c>
       <c r="AN81" t="s" s="2">
         <v>81</v>
       </c>
       <c r="AO81" t="s" s="2">
-        <v>535</v>
+        <v>536</v>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="s" s="2">
-        <v>536</v>
+        <v>537</v>
       </c>
       <c r="B82" t="s" s="2">
-        <v>536</v>
+        <v>537</v>
       </c>
       <c r="C82" s="2"/>
       <c r="D82" t="s" s="2">
@@ -11673,13 +11676,13 @@
         <v>81</v>
       </c>
       <c r="K82" t="s" s="2">
-        <v>496</v>
+        <v>497</v>
       </c>
       <c r="L82" t="s" s="2">
-        <v>537</v>
+        <v>538</v>
       </c>
       <c r="M82" t="s" s="2">
-        <v>538</v>
+        <v>539</v>
       </c>
       <c r="N82" s="2"/>
       <c r="O82" s="2"/>
@@ -11730,7 +11733,7 @@
         <v>81</v>
       </c>
       <c r="AF82" t="s" s="2">
-        <v>536</v>
+        <v>537</v>
       </c>
       <c r="AG82" t="s" s="2">
         <v>79</v>
@@ -11751,21 +11754,21 @@
         <v>81</v>
       </c>
       <c r="AM82" t="s" s="2">
-        <v>539</v>
+        <v>540</v>
       </c>
       <c r="AN82" t="s" s="2">
         <v>81</v>
       </c>
       <c r="AO82" t="s" s="2">
-        <v>540</v>
+        <v>541</v>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="s" s="2">
-        <v>541</v>
+        <v>542</v>
       </c>
       <c r="B83" t="s" s="2">
-        <v>541</v>
+        <v>542</v>
       </c>
       <c r="C83" s="2"/>
       <c r="D83" t="s" s="2">
@@ -11791,10 +11794,10 @@
         <v>225</v>
       </c>
       <c r="L83" t="s" s="2">
-        <v>542</v>
+        <v>543</v>
       </c>
       <c r="M83" t="s" s="2">
-        <v>543</v>
+        <v>544</v>
       </c>
       <c r="N83" s="2"/>
       <c r="O83" s="2"/>
@@ -11824,10 +11827,10 @@
         <v>323</v>
       </c>
       <c r="Y83" t="s" s="2">
-        <v>544</v>
+        <v>545</v>
       </c>
       <c r="Z83" t="s" s="2">
-        <v>545</v>
+        <v>546</v>
       </c>
       <c r="AA83" t="s" s="2">
         <v>81</v>
@@ -11845,7 +11848,7 @@
         <v>81</v>
       </c>
       <c r="AF83" t="s" s="2">
-        <v>541</v>
+        <v>542</v>
       </c>
       <c r="AG83" t="s" s="2">
         <v>79</v>
@@ -11866,21 +11869,21 @@
         <v>81</v>
       </c>
       <c r="AM83" t="s" s="2">
-        <v>546</v>
+        <v>547</v>
       </c>
       <c r="AN83" t="s" s="2">
         <v>81</v>
       </c>
       <c r="AO83" t="s" s="2">
-        <v>547</v>
+        <v>548</v>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="s" s="2">
-        <v>548</v>
+        <v>549</v>
       </c>
       <c r="B84" t="s" s="2">
-        <v>548</v>
+        <v>549</v>
       </c>
       <c r="C84" s="2"/>
       <c r="D84" t="s" s="2">
@@ -11906,13 +11909,13 @@
         <v>283</v>
       </c>
       <c r="L84" t="s" s="2">
-        <v>549</v>
+        <v>550</v>
       </c>
       <c r="M84" t="s" s="2">
-        <v>550</v>
+        <v>551</v>
       </c>
       <c r="N84" t="s" s="2">
-        <v>551</v>
+        <v>552</v>
       </c>
       <c r="O84" s="2"/>
       <c r="P84" t="s" s="2">
@@ -11962,7 +11965,7 @@
         <v>81</v>
       </c>
       <c r="AF84" t="s" s="2">
-        <v>548</v>
+        <v>549</v>
       </c>
       <c r="AG84" t="s" s="2">
         <v>79</v>
@@ -11983,7 +11986,7 @@
         <v>81</v>
       </c>
       <c r="AM84" t="s" s="2">
-        <v>552</v>
+        <v>553</v>
       </c>
       <c r="AN84" t="s" s="2">
         <v>81</v>
@@ -11994,10 +11997,10 @@
     </row>
     <row r="85">
       <c r="A85" t="s" s="2">
-        <v>553</v>
+        <v>554</v>
       </c>
       <c r="B85" t="s" s="2">
-        <v>553</v>
+        <v>554</v>
       </c>
       <c r="C85" s="2"/>
       <c r="D85" t="s" s="2">
@@ -12109,10 +12112,10 @@
     </row>
     <row r="86">
       <c r="A86" t="s" s="2">
-        <v>554</v>
+        <v>555</v>
       </c>
       <c r="B86" t="s" s="2">
-        <v>554</v>
+        <v>555</v>
       </c>
       <c r="C86" s="2"/>
       <c r="D86" t="s" s="2">
@@ -12226,10 +12229,10 @@
     </row>
     <row r="87">
       <c r="A87" t="s" s="2">
-        <v>555</v>
+        <v>556</v>
       </c>
       <c r="B87" t="s" s="2">
-        <v>555</v>
+        <v>556</v>
       </c>
       <c r="C87" s="2"/>
       <c r="D87" t="s" s="2">
@@ -12345,10 +12348,10 @@
     </row>
     <row r="88">
       <c r="A88" t="s" s="2">
-        <v>556</v>
+        <v>557</v>
       </c>
       <c r="B88" t="s" s="2">
-        <v>556</v>
+        <v>557</v>
       </c>
       <c r="C88" s="2"/>
       <c r="D88" t="s" s="2">
@@ -12371,13 +12374,13 @@
         <v>81</v>
       </c>
       <c r="K88" t="s" s="2">
-        <v>557</v>
+        <v>558</v>
       </c>
       <c r="L88" t="s" s="2">
-        <v>558</v>
+        <v>559</v>
       </c>
       <c r="M88" t="s" s="2">
-        <v>559</v>
+        <v>560</v>
       </c>
       <c r="N88" s="2"/>
       <c r="O88" s="2"/>
@@ -12428,7 +12431,7 @@
         <v>81</v>
       </c>
       <c r="AF88" t="s" s="2">
-        <v>556</v>
+        <v>557</v>
       </c>
       <c r="AG88" t="s" s="2">
         <v>90</v>
@@ -12446,24 +12449,24 @@
         <v>81</v>
       </c>
       <c r="AL88" t="s" s="2">
-        <v>560</v>
+        <v>561</v>
       </c>
       <c r="AM88" t="s" s="2">
         <v>394</v>
       </c>
       <c r="AN88" t="s" s="2">
-        <v>561</v>
+        <v>562</v>
       </c>
       <c r="AO88" t="s" s="2">
-        <v>562</v>
+        <v>563</v>
       </c>
     </row>
     <row r="89">
       <c r="A89" t="s" s="2">
-        <v>563</v>
+        <v>564</v>
       </c>
       <c r="B89" t="s" s="2">
-        <v>563</v>
+        <v>564</v>
       </c>
       <c r="C89" s="2"/>
       <c r="D89" t="s" s="2">
@@ -12489,13 +12492,13 @@
         <v>110</v>
       </c>
       <c r="L89" t="s" s="2">
-        <v>564</v>
+        <v>565</v>
       </c>
       <c r="M89" t="s" s="2">
-        <v>565</v>
+        <v>566</v>
       </c>
       <c r="N89" t="s" s="2">
-        <v>566</v>
+        <v>567</v>
       </c>
       <c r="O89" s="2"/>
       <c r="P89" t="s" s="2">
@@ -12524,10 +12527,10 @@
         <v>218</v>
       </c>
       <c r="Y89" t="s" s="2">
-        <v>567</v>
+        <v>568</v>
       </c>
       <c r="Z89" t="s" s="2">
-        <v>568</v>
+        <v>569</v>
       </c>
       <c r="AA89" t="s" s="2">
         <v>81</v>
@@ -12545,7 +12548,7 @@
         <v>81</v>
       </c>
       <c r="AF89" t="s" s="2">
-        <v>563</v>
+        <v>564</v>
       </c>
       <c r="AG89" t="s" s="2">
         <v>79</v>
@@ -12566,7 +12569,7 @@
         <v>81</v>
       </c>
       <c r="AM89" t="s" s="2">
-        <v>569</v>
+        <v>570</v>
       </c>
       <c r="AN89" t="s" s="2">
         <v>81</v>
@@ -12577,10 +12580,10 @@
     </row>
     <row r="90">
       <c r="A90" t="s" s="2">
-        <v>570</v>
+        <v>571</v>
       </c>
       <c r="B90" t="s" s="2">
-        <v>570</v>
+        <v>571</v>
       </c>
       <c r="C90" s="2"/>
       <c r="D90" t="s" s="2">
@@ -12606,13 +12609,13 @@
         <v>225</v>
       </c>
       <c r="L90" t="s" s="2">
-        <v>571</v>
+        <v>572</v>
       </c>
       <c r="M90" t="s" s="2">
-        <v>572</v>
+        <v>573</v>
       </c>
       <c r="N90" t="s" s="2">
-        <v>573</v>
+        <v>574</v>
       </c>
       <c r="O90" s="2"/>
       <c r="P90" t="s" s="2">
@@ -12641,10 +12644,10 @@
         <v>323</v>
       </c>
       <c r="Y90" t="s" s="2">
-        <v>574</v>
+        <v>575</v>
       </c>
       <c r="Z90" t="s" s="2">
-        <v>575</v>
+        <v>576</v>
       </c>
       <c r="AA90" t="s" s="2">
         <v>81</v>
@@ -12662,7 +12665,7 @@
         <v>81</v>
       </c>
       <c r="AF90" t="s" s="2">
-        <v>570</v>
+        <v>571</v>
       </c>
       <c r="AG90" t="s" s="2">
         <v>79</v>
@@ -12694,10 +12697,10 @@
     </row>
     <row r="91">
       <c r="A91" t="s" s="2">
-        <v>576</v>
+        <v>577</v>
       </c>
       <c r="B91" t="s" s="2">
-        <v>576</v>
+        <v>577</v>
       </c>
       <c r="C91" s="2"/>
       <c r="D91" t="s" s="2">
@@ -12723,10 +12726,10 @@
         <v>257</v>
       </c>
       <c r="L91" t="s" s="2">
-        <v>577</v>
+        <v>578</v>
       </c>
       <c r="M91" t="s" s="2">
-        <v>578</v>
+        <v>579</v>
       </c>
       <c r="N91" s="2"/>
       <c r="O91" s="2"/>
@@ -12777,7 +12780,7 @@
         <v>81</v>
       </c>
       <c r="AF91" t="s" s="2">
-        <v>576</v>
+        <v>577</v>
       </c>
       <c r="AG91" t="s" s="2">
         <v>79</v>
@@ -12809,10 +12812,10 @@
     </row>
     <row r="92">
       <c r="A92" t="s" s="2">
-        <v>579</v>
+        <v>580</v>
       </c>
       <c r="B92" t="s" s="2">
-        <v>579</v>
+        <v>580</v>
       </c>
       <c r="C92" s="2"/>
       <c r="D92" t="s" s="2">
@@ -12835,13 +12838,13 @@
         <v>81</v>
       </c>
       <c r="K92" t="s" s="2">
-        <v>580</v>
+        <v>581</v>
       </c>
       <c r="L92" t="s" s="2">
-        <v>581</v>
+        <v>582</v>
       </c>
       <c r="M92" t="s" s="2">
-        <v>582</v>
+        <v>583</v>
       </c>
       <c r="N92" s="2"/>
       <c r="O92" s="2"/>
@@ -12892,7 +12895,7 @@
         <v>81</v>
       </c>
       <c r="AF92" t="s" s="2">
-        <v>579</v>
+        <v>580</v>
       </c>
       <c r="AG92" t="s" s="2">
         <v>79</v>
@@ -12907,27 +12910,27 @@
         <v>102</v>
       </c>
       <c r="AK92" t="s" s="2">
-        <v>583</v>
+        <v>584</v>
       </c>
       <c r="AL92" t="s" s="2">
         <v>393</v>
       </c>
       <c r="AM92" t="s" s="2">
-        <v>584</v>
+        <v>585</v>
       </c>
       <c r="AN92" t="s" s="2">
         <v>81</v>
       </c>
       <c r="AO92" t="s" s="2">
-        <v>585</v>
+        <v>586</v>
       </c>
     </row>
     <row r="93">
       <c r="A93" t="s" s="2">
-        <v>586</v>
+        <v>587</v>
       </c>
       <c r="B93" t="s" s="2">
-        <v>586</v>
+        <v>587</v>
       </c>
       <c r="C93" s="2"/>
       <c r="D93" t="s" s="2">
@@ -12950,16 +12953,16 @@
         <v>81</v>
       </c>
       <c r="K93" t="s" s="2">
-        <v>587</v>
+        <v>588</v>
       </c>
       <c r="L93" t="s" s="2">
-        <v>588</v>
+        <v>589</v>
       </c>
       <c r="M93" t="s" s="2">
-        <v>589</v>
+        <v>590</v>
       </c>
       <c r="N93" t="s" s="2">
-        <v>590</v>
+        <v>591</v>
       </c>
       <c r="O93" s="2"/>
       <c r="P93" t="s" s="2">
@@ -13009,7 +13012,7 @@
         <v>81</v>
       </c>
       <c r="AF93" t="s" s="2">
-        <v>586</v>
+        <v>587</v>
       </c>
       <c r="AG93" t="s" s="2">
         <v>79</v>
@@ -13027,10 +13030,10 @@
         <v>81</v>
       </c>
       <c r="AL93" t="s" s="2">
-        <v>591</v>
+        <v>592</v>
       </c>
       <c r="AM93" t="s" s="2">
-        <v>592</v>
+        <v>593</v>
       </c>
       <c r="AN93" t="s" s="2">
         <v>81</v>

</xml_diff>